<commit_message>
Updating with today's lesson word list.
</commit_message>
<xml_diff>
--- a/data/Words1.xlsx
+++ b/data/Words1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
   <si>
     <t xml:space="preserve">Farsi</t>
   </si>
@@ -31,16 +31,190 @@
     <t xml:space="preserve">English</t>
   </si>
   <si>
-    <t xml:space="preserve">Meaning</t>
-  </si>
-  <si>
     <t xml:space="preserve">آتش</t>
   </si>
   <si>
-    <t xml:space="preserve">Ah tash</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fire</t>
+    <t xml:space="preserve">ah tash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ضعیف</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">اوج</t>
+  </si>
+  <si>
+    <t xml:space="preserve">top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">زحل</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saturn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">کلی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">general</t>
+  </si>
+  <si>
+    <t xml:space="preserve">حل کردن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to solve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">اجل</t>
+  </si>
+  <si>
+    <t xml:space="preserve">death</t>
+  </si>
+  <si>
+    <t xml:space="preserve">حیل</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gimmick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">لانه</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">آشوب</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chaos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">وسیع</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extensive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">هرج مرج</t>
+  </si>
+  <si>
+    <t xml:space="preserve">مواکز</t>
+  </si>
+  <si>
+    <t xml:space="preserve">centers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">آب ترین</t>
+  </si>
+  <si>
+    <t xml:space="preserve">most watery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">سر چشمه</t>
+  </si>
+  <si>
+    <t xml:space="preserve">source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">تقسیم</t>
+  </si>
+  <si>
+    <t xml:space="preserve">division</t>
+  </si>
+  <si>
+    <t xml:space="preserve">کارخانجات</t>
+  </si>
+  <si>
+    <t xml:space="preserve">factories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">تا سیسات</t>
+  </si>
+  <si>
+    <t xml:space="preserve">installations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">اداری</t>
+  </si>
+  <si>
+    <t xml:space="preserve">administrative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">صنعتی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">industrial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">نفت</t>
+  </si>
+  <si>
+    <t xml:space="preserve">olil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ملی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">national</t>
+  </si>
+  <si>
+    <t xml:space="preserve">حفاری</t>
+  </si>
+  <si>
+    <t xml:space="preserve">evacuation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ایراد</t>
+  </si>
+  <si>
+    <t xml:space="preserve">objection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">یا دآوری کردن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to notifiy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شبیه</t>
+  </si>
+  <si>
+    <t xml:space="preserve">similar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">گیتار</t>
+  </si>
+  <si>
+    <t xml:space="preserve">guitar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">سشکست حوردن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">کول</t>
+  </si>
+  <si>
+    <t xml:space="preserve">piggyback</t>
+  </si>
+  <si>
+    <t xml:space="preserve">دیگ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">دیوار</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wall</t>
   </si>
 </sst>
 </file>
@@ -119,12 +293,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -145,10 +323,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -163,22 +341,256 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>6</v>
+      <c r="C3" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed some spelling mistakes on the data file and confirmed that the basic play function is outputting what it's supposed to.
</commit_message>
<xml_diff>
--- a/data/Words1.xlsx
+++ b/data/Words1.xlsx
@@ -106,7 +106,7 @@
     <t xml:space="preserve">مواکز</t>
   </si>
   <si>
-    <t xml:space="preserve">centers</t>
+    <t xml:space="preserve">centres</t>
   </si>
   <si>
     <t xml:space="preserve">آب ترین</t>
@@ -154,7 +154,7 @@
     <t xml:space="preserve">نفت</t>
   </si>
   <si>
-    <t xml:space="preserve">olil</t>
+    <t xml:space="preserve">oil</t>
   </si>
   <si>
     <t xml:space="preserve">ملی</t>
@@ -178,7 +178,7 @@
     <t xml:space="preserve">یا دآوری کردن</t>
   </si>
   <si>
-    <t xml:space="preserve">to notifiy</t>
+    <t xml:space="preserve">to notify</t>
   </si>
   <si>
     <t xml:space="preserve">شبیه</t>
@@ -229,6 +229,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -249,6 +250,7 @@
       <sz val="10"/>
       <name val="Lohit Devanagari"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -298,11 +300,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -326,270 +328,270 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" s="1" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding more scoring output, and more words!
</commit_message>
<xml_diff>
--- a/data/Words1.xlsx
+++ b/data/Words1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="184">
   <si>
     <t xml:space="preserve">Farsi</t>
   </si>
@@ -215,6 +215,363 @@
   </si>
   <si>
     <t xml:space="preserve">wall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">بودن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boodan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">be</t>
+  </si>
+  <si>
+    <t xml:space="preserve">هست</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">there is</t>
+  </si>
+  <si>
+    <t xml:space="preserve">داشتن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dashtan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">have</t>
+  </si>
+  <si>
+    <t xml:space="preserve">کردن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kardan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">do</t>
+  </si>
+  <si>
+    <t xml:space="preserve">رفتن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">go</t>
+  </si>
+  <si>
+    <t xml:space="preserve">khastan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">want</t>
+  </si>
+  <si>
+    <t xml:space="preserve">توانستن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tavanestan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">can</t>
+  </si>
+  <si>
+    <t xml:space="preserve">لازم داشتن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lazem dashtan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">need</t>
+  </si>
+  <si>
+    <t xml:space="preserve">فکر کردن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fekr kardan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">think</t>
+  </si>
+  <si>
+    <t xml:space="preserve">دانستن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">danestan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">know</t>
+  </si>
+  <si>
+    <t xml:space="preserve">گفتن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">goftan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">say</t>
+  </si>
+  <si>
+    <t xml:space="preserve">دوست داشتن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">doost dashtan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">like</t>
+  </si>
+  <si>
+    <t xml:space="preserve">صحبت کردن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sohbat kardan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">speak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">یاد گرفتن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yad gereftan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">learn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">فهمیدن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fahmeedan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">understand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">که</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">that (I think that...)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">و </t>
+  </si>
+  <si>
+    <t xml:space="preserve">va</t>
+  </si>
+  <si>
+    <t xml:space="preserve">and</t>
+  </si>
+  <si>
+    <t xml:space="preserve">یا</t>
+  </si>
+  <si>
+    <t xml:space="preserve">or</t>
+  </si>
+  <si>
+    <t xml:space="preserve">امّا , ولی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Am-ma, vali</t>
+  </si>
+  <si>
+    <t xml:space="preserve">but</t>
+  </si>
+  <si>
+    <t xml:space="preserve">چون که</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chonke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">because</t>
+  </si>
+  <si>
+    <t xml:space="preserve">گرچه</t>
+  </si>
+  <si>
+    <t xml:space="preserve">garche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">though</t>
+  </si>
+  <si>
+    <t xml:space="preserve">بنابر این</t>
+  </si>
+  <si>
+    <t xml:space="preserve">banabar’een</t>
+  </si>
+  <si>
+    <t xml:space="preserve">اگر</t>
+  </si>
+  <si>
+    <t xml:space="preserve">agar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if</t>
+  </si>
+  <si>
+    <t xml:space="preserve">از</t>
+  </si>
+  <si>
+    <t xml:space="preserve">az</t>
+  </si>
+  <si>
+    <t xml:space="preserve">of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">به</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to </t>
+  </si>
+  <si>
+    <t xml:space="preserve">from</t>
+  </si>
+  <si>
+    <t xml:space="preserve">تو</t>
+  </si>
+  <si>
+    <t xml:space="preserve">too</t>
+  </si>
+  <si>
+    <t xml:space="preserve">توی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tooye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">at (a place)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">با</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ba </t>
+  </si>
+  <si>
+    <t xml:space="preserve">with</t>
+  </si>
+  <si>
+    <t xml:space="preserve">راجع به</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raje’be</t>
+  </si>
+  <si>
+    <t xml:space="preserve">about</t>
+  </si>
+  <si>
+    <t xml:space="preserve">مثل</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mesle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">برای</t>
+  </si>
+  <si>
+    <t xml:space="preserve">baraye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for</t>
+  </si>
+  <si>
+    <t xml:space="preserve">قبل از</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ghabl az</t>
+  </si>
+  <si>
+    <t xml:space="preserve">before</t>
+  </si>
+  <si>
+    <t xml:space="preserve">بعد از</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ba’d az</t>
+  </si>
+  <si>
+    <t xml:space="preserve">after</t>
+  </si>
+  <si>
+    <t xml:space="preserve">در حین</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dar heyne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">during</t>
+  </si>
+  <si>
+    <t xml:space="preserve">کی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">who</t>
+  </si>
+  <si>
+    <t xml:space="preserve">چی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">what</t>
+  </si>
+  <si>
+    <t xml:space="preserve">کجا</t>
+  </si>
+  <si>
+    <t xml:space="preserve">koja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">where</t>
+  </si>
+  <si>
+    <t xml:space="preserve">key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">when</t>
+  </si>
+  <si>
+    <t xml:space="preserve">چرا</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">why</t>
+  </si>
+  <si>
+    <t xml:space="preserve">چطور/ چطور</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chegooneh/chetor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">how</t>
+  </si>
+  <si>
+    <t xml:space="preserve">چقدر</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cheghad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">how much</t>
+  </si>
+  <si>
+    <t xml:space="preserve">کدام</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kodam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">which</t>
   </si>
 </sst>
 </file>
@@ -224,7 +581,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -249,6 +606,13 @@
     <font>
       <sz val="10"/>
       <name val="Lohit Devanagari"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -295,7 +659,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -306,6 +670,18 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -325,13 +701,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C77" activeCellId="0" sqref="C77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -593,6 +969,479 @@
       </c>
       <c r="C32" s="1" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
150+ words now - planni ng on failure output/store.
</commit_message>
<xml_diff>
--- a/data/Words1.xlsx
+++ b/data/Words1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="399">
   <si>
     <t xml:space="preserve">Farsi</t>
   </si>
@@ -938,16 +938,296 @@
   </si>
   <si>
     <t xml:space="preserve">bit of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">most  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">دیگر</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deegar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">یکی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yeki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">same</t>
+  </si>
+  <si>
+    <t xml:space="preserve">مختلف</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mokhtalef</t>
+  </si>
+  <si>
+    <t xml:space="preserve">different</t>
+  </si>
+  <si>
+    <t xml:space="preserve">کافی :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">دو</t>
+  </si>
+  <si>
+    <t xml:space="preserve">do </t>
+  </si>
+  <si>
+    <t xml:space="preserve">two</t>
+  </si>
+  <si>
+    <t xml:space="preserve">تعداد کمی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">te’dade kami</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a few</t>
+  </si>
+  <si>
+    <t xml:space="preserve">اوّلی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Av-vali</t>
+  </si>
+  <si>
+    <t xml:space="preserve">first</t>
+  </si>
+  <si>
+    <t xml:space="preserve">بعدی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ba’di</t>
+  </si>
+  <si>
+    <t xml:space="preserve">next</t>
+  </si>
+  <si>
+    <t xml:space="preserve">آخری</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ghabli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">last</t>
+  </si>
+  <si>
+    <t xml:space="preserve">akhari</t>
+  </si>
+  <si>
+    <t xml:space="preserve">راحت</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rahat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">easy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">سخت</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sakht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">زود</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">early</t>
+  </si>
+  <si>
+    <t xml:space="preserve">دیر</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">late</t>
+  </si>
+  <si>
+    <t xml:space="preserve">مهمّ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mohemm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">important</t>
+  </si>
+  <si>
+    <t xml:space="preserve">جالب</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jaleb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interesting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">باحال</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bahal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">حوصله سر بر</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hosele sar bar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">زیبا</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zeeba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beautiful</t>
+  </si>
+  <si>
+    <t xml:space="preserve">بزرگ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bozorg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">big</t>
+  </si>
+  <si>
+    <t xml:space="preserve">کوچک</t>
+  </si>
+  <si>
+    <t xml:space="preserve">koochack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">small</t>
+  </si>
+  <si>
+    <t xml:space="preserve">خوشحال</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kohosh-hal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">happy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ناراحت</t>
+  </si>
+  <si>
+    <t xml:space="preserve">narahat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">مشغول</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mashghool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">busy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">هیجان داشتن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hayejan dashtan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to be excited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">خسته</t>
+  </si>
+  <si>
+    <t xml:space="preserve">khaste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tired</t>
+  </si>
+  <si>
+    <t xml:space="preserve">آماده</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ready</t>
+  </si>
+  <si>
+    <t xml:space="preserve">مورد علاقهجدید</t>
+  </si>
+  <si>
+    <t xml:space="preserve">morede alaghe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">favourite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">جدید</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jadid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new</t>
+  </si>
+  <si>
+    <t xml:space="preserve">درست</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dorost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">اشتباه</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eshtebah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wrong</t>
+  </si>
+  <si>
+    <t xml:space="preserve">راست</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rast</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -972,13 +1252,6 @@
     <font>
       <sz val="10"/>
       <name val="Lohit Devanagari"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -1046,8 +1319,8 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1067,13 +1340,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C122"/>
+  <dimension ref="A1:C156"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A107" colorId="64" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F113" activeCellId="0" sqref="F113"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="11.59"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1337,7 +1613,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
         <v>65</v>
       </c>
@@ -1348,7 +1624,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
         <v>68</v>
       </c>
@@ -1359,7 +1635,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
         <v>71</v>
       </c>
@@ -1370,7 +1646,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
         <v>74</v>
       </c>
@@ -1381,7 +1657,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
         <v>77</v>
       </c>
@@ -1392,7 +1668,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
         <v>77</v>
       </c>
@@ -1403,7 +1679,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
         <v>81</v>
       </c>
@@ -1414,7 +1690,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
         <v>84</v>
       </c>
@@ -1425,7 +1701,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
         <v>87</v>
       </c>
@@ -1436,7 +1712,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
         <v>90</v>
       </c>
@@ -1447,7 +1723,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
         <v>93</v>
       </c>
@@ -1458,7 +1734,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
         <v>96</v>
       </c>
@@ -1469,7 +1745,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
         <v>99</v>
       </c>
@@ -1480,7 +1756,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
         <v>102</v>
       </c>
@@ -1491,7 +1767,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
         <v>105</v>
       </c>
@@ -1591,7 +1867,7 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="5" t="s">
+      <c r="A56" s="3" t="s">
         <v>130</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -1602,7 +1878,7 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="5" t="s">
+      <c r="A57" s="3" t="s">
         <v>133</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -1613,7 +1889,7 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="5" t="s">
+      <c r="A58" s="3" t="s">
         <v>130</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -1624,7 +1900,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="5" t="s">
+      <c r="A59" s="3" t="s">
         <v>136</v>
       </c>
       <c r="B59" s="1" t="s">
@@ -1635,7 +1911,7 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="5" t="s">
+      <c r="A60" s="3" t="s">
         <v>138</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -1646,7 +1922,7 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="5" t="s">
+      <c r="A61" s="3" t="s">
         <v>141</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -1657,7 +1933,7 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="5" t="s">
+      <c r="A62" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B62" s="1" t="s">
@@ -1668,7 +1944,7 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="5" t="s">
+      <c r="A63" s="3" t="s">
         <v>147</v>
       </c>
       <c r="B63" s="1" t="s">
@@ -1679,7 +1955,7 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="5" t="s">
+      <c r="A64" s="3" t="s">
         <v>149</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -1690,7 +1966,7 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="5" t="s">
+      <c r="A65" s="3" t="s">
         <v>152</v>
       </c>
       <c r="B65" s="1" t="s">
@@ -1701,7 +1977,7 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="5" t="s">
+      <c r="A66" s="3" t="s">
         <v>155</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -1712,7 +1988,7 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="5" t="s">
+      <c r="A67" s="3" t="s">
         <v>158</v>
       </c>
       <c r="B67" s="1" t="s">
@@ -1723,7 +1999,7 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="5" t="s">
+      <c r="A68" s="3" t="s">
         <v>161</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -1734,7 +2010,7 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="5" t="s">
+      <c r="A69" s="3" t="s">
         <v>164</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -1745,7 +2021,7 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="5" t="s">
+      <c r="A70" s="3" t="s">
         <v>167</v>
       </c>
       <c r="B70" s="1" t="s">
@@ -1811,520 +2087,894 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="5" t="s">
+      <c r="A76" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="B76" s="0" t="s">
+      <c r="B76" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C76" s="0" t="s">
+      <c r="C76" s="1" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="5" t="s">
+      <c r="A77" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="B77" s="0" t="s">
+      <c r="B77" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="C77" s="0" t="s">
+      <c r="C77" s="1" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="5" t="s">
+      <c r="A78" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="B78" s="0" t="s">
+      <c r="B78" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="C78" s="0" t="s">
+      <c r="C78" s="1" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="5" t="s">
+      <c r="A79" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="B79" s="0" t="s">
+      <c r="B79" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C79" s="0" t="s">
+      <c r="C79" s="1" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="5" t="s">
+      <c r="A80" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="B80" s="0" t="s">
+      <c r="B80" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="C80" s="0" t="s">
+      <c r="C80" s="1" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="5" t="s">
+      <c r="A81" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="B81" s="0" t="s">
+      <c r="B81" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C81" s="0" t="s">
+      <c r="C81" s="1" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="5" t="s">
+      <c r="A82" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="B82" s="0" t="s">
+      <c r="B82" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="C82" s="0" t="s">
+      <c r="C82" s="1" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="5" t="s">
+      <c r="A83" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="B83" s="0" t="s">
+      <c r="B83" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C83" s="0" t="s">
+      <c r="C83" s="1" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="5" t="s">
+      <c r="A84" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="B84" s="0" t="s">
+      <c r="B84" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C84" s="0" t="s">
+      <c r="C84" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="5" t="s">
+      <c r="A85" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="B85" s="0" t="s">
+      <c r="B85" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C85" s="0" t="s">
+      <c r="C85" s="1" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="5" t="s">
+      <c r="A86" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="B86" s="0" t="s">
+      <c r="B86" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C86" s="0" t="s">
+      <c r="C86" s="1" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="5" t="s">
+      <c r="A87" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="B87" s="0" t="s">
+      <c r="B87" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C87" s="0" t="s">
+      <c r="C87" s="1" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="5" t="s">
+      <c r="A88" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="B88" s="0" t="s">
+      <c r="B88" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C88" s="0" t="s">
+      <c r="C88" s="1" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="5" t="s">
+      <c r="A89" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="B89" s="0" t="s">
+      <c r="B89" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C89" s="0" t="s">
+      <c r="C89" s="1" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="5" t="s">
+      <c r="A90" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="B90" s="0" t="s">
+      <c r="B90" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C90" s="0" t="s">
+      <c r="C90" s="1" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="5" t="s">
+      <c r="A91" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="B91" s="0" t="s">
+      <c r="B91" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="C91" s="0" t="s">
+      <c r="C91" s="1" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="5" t="s">
+      <c r="A92" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="B92" s="0" t="s">
+      <c r="B92" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="C92" s="0" t="s">
+      <c r="C92" s="1" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="5" t="s">
+      <c r="A93" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="B93" s="0" t="s">
+      <c r="B93" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="C93" s="0" t="s">
+      <c r="C93" s="1" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="5" t="s">
+      <c r="A94" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="B94" s="0" t="s">
+      <c r="B94" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="C94" s="0" t="s">
+      <c r="C94" s="1" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="5" t="s">
+      <c r="A95" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="B95" s="0" t="s">
+      <c r="B95" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C95" s="0" t="s">
+      <c r="C95" s="1" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="5" t="s">
+      <c r="A96" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="B96" s="0" t="s">
+      <c r="B96" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="C96" s="0" t="s">
+      <c r="C96" s="1" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="5" t="s">
+      <c r="A97" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="B97" s="0" t="s">
+      <c r="B97" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="C97" s="0" t="s">
+      <c r="C97" s="1" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="5" t="s">
+      <c r="A98" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="B98" s="0" t="s">
+      <c r="B98" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C98" s="0" t="s">
+      <c r="C98" s="1" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="5" t="s">
+      <c r="A99" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="B99" s="0" t="s">
+      <c r="B99" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="C99" s="0" t="s">
+      <c r="C99" s="1" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="5" t="s">
+      <c r="A100" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="B100" s="0" t="s">
+      <c r="B100" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="C100" s="0" t="s">
+      <c r="C100" s="1" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="5" t="s">
+      <c r="A101" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="B101" s="0" t="s">
+      <c r="B101" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="C101" s="0" t="s">
+      <c r="C101" s="1" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="5" t="s">
+      <c r="A102" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="B102" s="0" t="s">
+      <c r="B102" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="C102" s="0" t="s">
+      <c r="C102" s="1" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="5" t="s">
+      <c r="A103" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="B103" s="0" t="s">
+      <c r="B103" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="C103" s="0" t="s">
+      <c r="C103" s="1" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="5" t="s">
+      <c r="A104" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="B104" s="0" t="s">
+      <c r="B104" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="C104" s="0" t="s">
+      <c r="C104" s="1" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="5" t="s">
+      <c r="A105" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="B105" s="0" t="s">
+      <c r="B105" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="C105" s="0" t="s">
+      <c r="C105" s="1" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="5" t="s">
+      <c r="A106" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="B106" s="0" t="s">
+      <c r="B106" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="C106" s="0" t="s">
+      <c r="C106" s="1" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="5" t="s">
+      <c r="A107" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="B107" s="0" t="s">
+      <c r="B107" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="C107" s="0" t="s">
+      <c r="C107" s="1" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A108" s="5" t="s">
+      <c r="A108" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="B108" s="0" t="s">
+      <c r="B108" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="C108" s="0" t="s">
+      <c r="C108" s="1" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="5" t="s">
+      <c r="A109" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="B109" s="0" t="s">
+      <c r="B109" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C109" s="0" t="s">
+      <c r="C109" s="1" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="5" t="s">
+      <c r="A110" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="B110" s="0" t="s">
+      <c r="B110" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="C110" s="0" t="s">
+      <c r="C110" s="1" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="5" t="s">
+      <c r="A111" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="B111" s="0" t="s">
+      <c r="B111" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="C111" s="0" t="s">
+      <c r="C111" s="1" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="5" t="s">
+      <c r="A112" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="B112" s="0" t="s">
+      <c r="B112" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="C112" s="0" t="s">
+      <c r="C112" s="1" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="5" t="s">
+      <c r="A113" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="B113" s="0" t="s">
+      <c r="B113" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C113" s="0" t="s">
+      <c r="C113" s="1" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="5" t="s">
+      <c r="A114" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="B114" s="0" t="s">
+      <c r="B114" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="C114" s="0" t="s">
+      <c r="C114" s="1" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="5" t="s">
+      <c r="A115" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="B115" s="0" t="s">
+      <c r="B115" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="C115" s="0" t="s">
+      <c r="C115" s="1" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="5" t="s">
+      <c r="A116" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="B116" s="0" t="s">
+      <c r="B116" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C116" s="0" t="s">
+      <c r="C116" s="1" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="5" t="s">
+      <c r="A117" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="B117" s="0" t="s">
+      <c r="B117" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="C117" s="0" t="s">
+      <c r="C117" s="1" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="5" t="s">
+      <c r="A118" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="B118" s="0" t="s">
+      <c r="B118" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="C118" s="0" t="s">
+      <c r="C118" s="1" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="5" t="s">
+      <c r="A119" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="B119" s="0" t="s">
+      <c r="B119" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="C119" s="0" t="s">
+      <c r="C119" s="1" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="5" t="s">
+      <c r="A120" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="B120" s="0" t="s">
+      <c r="B120" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="C120" s="0" t="s">
+      <c r="C120" s="1" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="5" t="s">
+      <c r="A121" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="B121" s="0" t="s">
+      <c r="B121" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="C121" s="0" t="s">
+      <c r="C121" s="1" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="5" t="s">
+      <c r="A122" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="B122" s="0" t="s">
+      <c r="B122" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="C122" s="0" t="s">
+      <c r="C122" s="1" t="s">
         <v>305</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C156" s="5" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Word update, logging failed words
</commit_message>
<xml_diff>
--- a/data/Words1.xlsx
+++ b/data/Words1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="402">
   <si>
     <t xml:space="preserve">Farsi</t>
   </si>
@@ -154,6 +154,9 @@
     <t xml:space="preserve">نفت</t>
   </si>
   <si>
+    <t xml:space="preserve">naft</t>
+  </si>
+  <si>
     <t xml:space="preserve">oil</t>
   </si>
   <si>
@@ -190,6 +193,9 @@
     <t xml:space="preserve">گیتار</t>
   </si>
   <si>
+    <t xml:space="preserve">gitar</t>
+  </si>
+  <si>
     <t xml:space="preserve">guitar</t>
   </si>
   <si>
@@ -206,6 +212,9 @@
   </si>
   <si>
     <t xml:space="preserve">دیگ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dig</t>
   </si>
   <si>
     <t xml:space="preserve">pot</t>
@@ -1342,8 +1351,8 @@
   </sheetPr>
   <dimension ref="A1:C156"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1529,327 +1538,336 @@
       <c r="A22" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="B22" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="C22" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>32</v>
@@ -1857,54 +1875,54 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>42</v>
@@ -1912,274 +1930,274 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="3" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="3" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="3" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="3" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="3" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="3" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>32</v>
@@ -2187,791 +2205,791 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="3" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="3" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="3" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="3" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="3" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="3" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="3" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="3" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="3" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="3" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="3" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="3" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="3" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="3" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="3" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="3" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="3" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="3" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="3" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="3" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="3" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="3" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="3" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="3" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="3" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="3" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="3" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="3" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="3" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="3" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="3" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="3" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="3" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="3" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="3" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="3" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="3" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="3" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="3" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="3" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="3" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="3" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="3" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="3" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="3" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="3" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="3" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="3" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="3" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="3" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="3" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="3" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="3" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="3" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="3" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="3" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="3" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="3" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="3" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="3" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="3" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="3" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="3" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="3" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="3" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="3" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="3" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="3" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="3" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="3" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="3" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="C156" s="5" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Moar words for Ba'al!
</commit_message>
<xml_diff>
--- a/data/Words1.xlsx
+++ b/data/Words1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="549">
   <si>
     <t xml:space="preserve">Farsi</t>
   </si>
@@ -1619,6 +1619,54 @@
   </si>
   <si>
     <t xml:space="preserve">Easy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">من</t>
+  </si>
+  <si>
+    <t xml:space="preserve">man </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I </t>
+  </si>
+  <si>
+    <t xml:space="preserve">you </t>
+  </si>
+  <si>
+    <t xml:space="preserve">او</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s/he</t>
+  </si>
+  <si>
+    <t xml:space="preserve">این/اون</t>
+  </si>
+  <si>
+    <t xml:space="preserve">een/oon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this/that</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ما</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شما</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shoma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">آنها</t>
+  </si>
+  <si>
+    <t xml:space="preserve">anha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">they</t>
   </si>
 </sst>
 </file>
@@ -1742,10 +1790,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C226"/>
+  <dimension ref="A1:C233"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A217" colorId="64" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C220" activeCellId="0" sqref="C220"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A222" colorId="64" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B233" activeCellId="0" sqref="B233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3393,7 +3441,6 @@
       <c r="A157" s="3" t="s">
         <v>402</v>
       </c>
-      <c r="B157" s="0"/>
       <c r="C157" s="3" t="s">
         <v>403</v>
       </c>
@@ -3402,7 +3449,6 @@
       <c r="A158" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="B158" s="0"/>
       <c r="C158" s="3" t="s">
         <v>405</v>
       </c>
@@ -3411,7 +3457,6 @@
       <c r="A159" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="B159" s="0"/>
       <c r="C159" s="3" t="s">
         <v>407</v>
       </c>
@@ -3420,7 +3465,6 @@
       <c r="A160" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="B160" s="0"/>
       <c r="C160" s="3" t="s">
         <v>409</v>
       </c>
@@ -3429,7 +3473,6 @@
       <c r="A161" s="3" t="s">
         <v>410</v>
       </c>
-      <c r="B161" s="0"/>
       <c r="C161" s="3" t="s">
         <v>411</v>
       </c>
@@ -3438,7 +3481,6 @@
       <c r="A162" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="B162" s="0"/>
       <c r="C162" s="3" t="s">
         <v>413</v>
       </c>
@@ -3447,7 +3489,6 @@
       <c r="A163" s="3" t="s">
         <v>414</v>
       </c>
-      <c r="B163" s="0"/>
       <c r="C163" s="3" t="s">
         <v>415</v>
       </c>
@@ -3456,7 +3497,6 @@
       <c r="A164" s="3" t="s">
         <v>416</v>
       </c>
-      <c r="B164" s="0"/>
       <c r="C164" s="3" t="s">
         <v>417</v>
       </c>
@@ -3465,7 +3505,6 @@
       <c r="A165" s="3" t="s">
         <v>418</v>
       </c>
-      <c r="B165" s="0"/>
       <c r="C165" s="3" t="s">
         <v>419</v>
       </c>
@@ -3474,7 +3513,6 @@
       <c r="A166" s="3" t="s">
         <v>420</v>
       </c>
-      <c r="B166" s="0"/>
       <c r="C166" s="3" t="s">
         <v>421</v>
       </c>
@@ -3483,7 +3521,6 @@
       <c r="A167" s="3" t="s">
         <v>422</v>
       </c>
-      <c r="B167" s="0"/>
       <c r="C167" s="3" t="s">
         <v>423</v>
       </c>
@@ -3492,7 +3529,6 @@
       <c r="A168" s="3" t="s">
         <v>424</v>
       </c>
-      <c r="B168" s="0"/>
       <c r="C168" s="3" t="s">
         <v>425</v>
       </c>
@@ -3501,7 +3537,6 @@
       <c r="A169" s="3" t="s">
         <v>426</v>
       </c>
-      <c r="B169" s="0"/>
       <c r="C169" s="3" t="s">
         <v>427</v>
       </c>
@@ -3510,7 +3545,6 @@
       <c r="A170" s="3" t="s">
         <v>428</v>
       </c>
-      <c r="B170" s="0"/>
       <c r="C170" s="3" t="s">
         <v>429</v>
       </c>
@@ -3519,7 +3553,6 @@
       <c r="A171" s="3" t="s">
         <v>430</v>
       </c>
-      <c r="B171" s="0"/>
       <c r="C171" s="3" t="s">
         <v>431</v>
       </c>
@@ -3528,7 +3561,6 @@
       <c r="A172" s="3" t="s">
         <v>432</v>
       </c>
-      <c r="B172" s="0"/>
       <c r="C172" s="3" t="s">
         <v>433</v>
       </c>
@@ -3537,7 +3569,6 @@
       <c r="A173" s="3" t="s">
         <v>434</v>
       </c>
-      <c r="B173" s="0"/>
       <c r="C173" s="3" t="s">
         <v>435</v>
       </c>
@@ -3546,7 +3577,6 @@
       <c r="A174" s="3" t="s">
         <v>436</v>
       </c>
-      <c r="B174" s="0"/>
       <c r="C174" s="3" t="s">
         <v>437</v>
       </c>
@@ -3555,7 +3585,6 @@
       <c r="A175" s="3" t="s">
         <v>438</v>
       </c>
-      <c r="B175" s="0"/>
       <c r="C175" s="3" t="s">
         <v>439</v>
       </c>
@@ -3564,7 +3593,6 @@
       <c r="A176" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="B176" s="0"/>
       <c r="C176" s="3" t="s">
         <v>440</v>
       </c>
@@ -3573,7 +3601,6 @@
       <c r="A177" s="3" t="s">
         <v>441</v>
       </c>
-      <c r="B177" s="0"/>
       <c r="C177" s="3" t="s">
         <v>442</v>
       </c>
@@ -3582,7 +3609,6 @@
       <c r="A178" s="3" t="s">
         <v>443</v>
       </c>
-      <c r="B178" s="0"/>
       <c r="C178" s="3" t="s">
         <v>444</v>
       </c>
@@ -3591,7 +3617,6 @@
       <c r="A179" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="B179" s="0"/>
       <c r="C179" s="3" t="s">
         <v>446</v>
       </c>
@@ -3600,7 +3625,6 @@
       <c r="A180" s="3" t="s">
         <v>447</v>
       </c>
-      <c r="B180" s="0"/>
       <c r="C180" s="3" t="s">
         <v>448</v>
       </c>
@@ -3609,7 +3633,6 @@
       <c r="A181" s="3" t="s">
         <v>449</v>
       </c>
-      <c r="B181" s="0"/>
       <c r="C181" s="3" t="s">
         <v>450</v>
       </c>
@@ -3618,7 +3641,6 @@
       <c r="A182" s="3" t="s">
         <v>451</v>
       </c>
-      <c r="B182" s="0"/>
       <c r="C182" s="3" t="s">
         <v>452</v>
       </c>
@@ -3627,7 +3649,6 @@
       <c r="A183" s="3" t="s">
         <v>453</v>
       </c>
-      <c r="B183" s="0"/>
       <c r="C183" s="3" t="s">
         <v>454</v>
       </c>
@@ -3636,7 +3657,6 @@
       <c r="A184" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="B184" s="0"/>
       <c r="C184" s="3" t="s">
         <v>456</v>
       </c>
@@ -3645,7 +3665,6 @@
       <c r="A185" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="B185" s="0"/>
       <c r="C185" s="3" t="s">
         <v>458</v>
       </c>
@@ -3654,7 +3673,6 @@
       <c r="A186" s="3" t="s">
         <v>459</v>
       </c>
-      <c r="B186" s="0"/>
       <c r="C186" s="3" t="s">
         <v>460</v>
       </c>
@@ -3663,7 +3681,6 @@
       <c r="A187" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="B187" s="0"/>
       <c r="C187" s="3" t="s">
         <v>462</v>
       </c>
@@ -3672,7 +3689,6 @@
       <c r="A188" s="3" t="s">
         <v>463</v>
       </c>
-      <c r="B188" s="0"/>
       <c r="C188" s="3" t="s">
         <v>464</v>
       </c>
@@ -3681,7 +3697,6 @@
       <c r="A189" s="3" t="s">
         <v>465</v>
       </c>
-      <c r="B189" s="0"/>
       <c r="C189" s="3" t="s">
         <v>466</v>
       </c>
@@ -3690,7 +3705,6 @@
       <c r="A190" s="3" t="s">
         <v>467</v>
       </c>
-      <c r="B190" s="0"/>
       <c r="C190" s="3" t="s">
         <v>468</v>
       </c>
@@ -3699,7 +3713,6 @@
       <c r="A191" s="3" t="s">
         <v>469</v>
       </c>
-      <c r="B191" s="0"/>
       <c r="C191" s="3" t="s">
         <v>470</v>
       </c>
@@ -3708,7 +3721,6 @@
       <c r="A192" s="3" t="s">
         <v>471</v>
       </c>
-      <c r="B192" s="0"/>
       <c r="C192" s="3" t="s">
         <v>472</v>
       </c>
@@ -3717,7 +3729,6 @@
       <c r="A193" s="3" t="s">
         <v>473</v>
       </c>
-      <c r="B193" s="0"/>
       <c r="C193" s="3" t="s">
         <v>474</v>
       </c>
@@ -3726,7 +3737,6 @@
       <c r="A194" s="3" t="s">
         <v>475</v>
       </c>
-      <c r="B194" s="0"/>
       <c r="C194" s="3" t="s">
         <v>476</v>
       </c>
@@ -3735,7 +3745,6 @@
       <c r="A195" s="3" t="s">
         <v>477</v>
       </c>
-      <c r="B195" s="0"/>
       <c r="C195" s="3" t="s">
         <v>478</v>
       </c>
@@ -3744,7 +3753,6 @@
       <c r="A196" s="3" t="s">
         <v>479</v>
       </c>
-      <c r="B196" s="0"/>
       <c r="C196" s="3" t="s">
         <v>480</v>
       </c>
@@ -3753,7 +3761,6 @@
       <c r="A197" s="3" t="s">
         <v>481</v>
       </c>
-      <c r="B197" s="0"/>
       <c r="C197" s="3" t="s">
         <v>482</v>
       </c>
@@ -3762,7 +3769,6 @@
       <c r="A198" s="3" t="s">
         <v>483</v>
       </c>
-      <c r="B198" s="0"/>
       <c r="C198" s="3" t="s">
         <v>484</v>
       </c>
@@ -3771,7 +3777,6 @@
       <c r="A199" s="3" t="s">
         <v>485</v>
       </c>
-      <c r="B199" s="0"/>
       <c r="C199" s="3" t="s">
         <v>486</v>
       </c>
@@ -3780,7 +3785,6 @@
       <c r="A200" s="3" t="s">
         <v>487</v>
       </c>
-      <c r="B200" s="0"/>
       <c r="C200" s="3" t="s">
         <v>488</v>
       </c>
@@ -3789,7 +3793,6 @@
       <c r="A201" s="3" t="s">
         <v>489</v>
       </c>
-      <c r="B201" s="0"/>
       <c r="C201" s="3" t="s">
         <v>490</v>
       </c>
@@ -3798,7 +3801,6 @@
       <c r="A202" s="3" t="s">
         <v>491</v>
       </c>
-      <c r="B202" s="0"/>
       <c r="C202" s="3" t="s">
         <v>492</v>
       </c>
@@ -3807,7 +3809,6 @@
       <c r="A203" s="3" t="s">
         <v>493</v>
       </c>
-      <c r="B203" s="0"/>
       <c r="C203" s="3" t="s">
         <v>494</v>
       </c>
@@ -3816,7 +3817,6 @@
       <c r="A204" s="3" t="s">
         <v>495</v>
       </c>
-      <c r="B204" s="0"/>
       <c r="C204" s="3" t="s">
         <v>496</v>
       </c>
@@ -3825,7 +3825,6 @@
       <c r="A205" s="3" t="s">
         <v>497</v>
       </c>
-      <c r="B205" s="0"/>
       <c r="C205" s="3" t="s">
         <v>498</v>
       </c>
@@ -3834,7 +3833,6 @@
       <c r="A206" s="3" t="s">
         <v>499</v>
       </c>
-      <c r="B206" s="0"/>
       <c r="C206" s="3" t="s">
         <v>500</v>
       </c>
@@ -3843,7 +3841,6 @@
       <c r="A207" s="3" t="s">
         <v>501</v>
       </c>
-      <c r="B207" s="0"/>
       <c r="C207" s="3" t="s">
         <v>502</v>
       </c>
@@ -3852,7 +3849,6 @@
       <c r="A208" s="3" t="s">
         <v>503</v>
       </c>
-      <c r="B208" s="0"/>
       <c r="C208" s="3" t="s">
         <v>504</v>
       </c>
@@ -3861,7 +3857,6 @@
       <c r="A209" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="B209" s="0"/>
       <c r="C209" s="3" t="s">
         <v>505</v>
       </c>
@@ -3870,7 +3865,6 @@
       <c r="A210" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B210" s="0"/>
       <c r="C210" s="3" t="s">
         <v>506</v>
       </c>
@@ -3879,7 +3873,6 @@
       <c r="A211" s="3" t="s">
         <v>507</v>
       </c>
-      <c r="B211" s="0"/>
       <c r="C211" s="3" t="s">
         <v>508</v>
       </c>
@@ -3888,7 +3881,6 @@
       <c r="A212" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="B212" s="0"/>
       <c r="C212" s="3" t="s">
         <v>509</v>
       </c>
@@ -3897,7 +3889,6 @@
       <c r="A213" s="3" t="s">
         <v>510</v>
       </c>
-      <c r="B213" s="0"/>
       <c r="C213" s="3" t="s">
         <v>511</v>
       </c>
@@ -3906,7 +3897,6 @@
       <c r="A214" s="3" t="s">
         <v>512</v>
       </c>
-      <c r="B214" s="0"/>
       <c r="C214" s="3" t="s">
         <v>513</v>
       </c>
@@ -3915,7 +3905,6 @@
       <c r="A215" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="B215" s="0"/>
       <c r="C215" s="3" t="s">
         <v>514</v>
       </c>
@@ -3924,7 +3913,6 @@
       <c r="A216" s="3" t="s">
         <v>515</v>
       </c>
-      <c r="B216" s="0"/>
       <c r="C216" s="3" t="s">
         <v>516</v>
       </c>
@@ -3933,7 +3921,6 @@
       <c r="A217" s="3" t="s">
         <v>517</v>
       </c>
-      <c r="B217" s="0"/>
       <c r="C217" s="3" t="s">
         <v>518</v>
       </c>
@@ -3942,7 +3929,6 @@
       <c r="A218" s="3" t="s">
         <v>519</v>
       </c>
-      <c r="B218" s="0"/>
       <c r="C218" s="3" t="s">
         <v>520</v>
       </c>
@@ -3951,7 +3937,6 @@
       <c r="A219" s="3" t="s">
         <v>521</v>
       </c>
-      <c r="B219" s="0"/>
       <c r="C219" s="3" t="s">
         <v>522</v>
       </c>
@@ -3960,7 +3945,6 @@
       <c r="A220" s="3" t="s">
         <v>523</v>
       </c>
-      <c r="B220" s="0"/>
       <c r="C220" s="3" t="s">
         <v>524</v>
       </c>
@@ -3969,7 +3953,6 @@
       <c r="A221" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="B221" s="0"/>
       <c r="C221" s="3" t="s">
         <v>525</v>
       </c>
@@ -3978,7 +3961,6 @@
       <c r="A222" s="3" t="s">
         <v>394</v>
       </c>
-      <c r="B222" s="0"/>
       <c r="C222" s="3" t="s">
         <v>526</v>
       </c>
@@ -3987,7 +3969,6 @@
       <c r="A223" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="B223" s="0"/>
       <c r="C223" s="3" t="s">
         <v>527</v>
       </c>
@@ -3996,7 +3977,6 @@
       <c r="A224" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="B224" s="0"/>
       <c r="C224" s="3" t="s">
         <v>528</v>
       </c>
@@ -4005,7 +3985,6 @@
       <c r="A225" s="3" t="s">
         <v>529</v>
       </c>
-      <c r="B225" s="0"/>
       <c r="C225" s="3" t="s">
         <v>530</v>
       </c>
@@ -4014,9 +3993,85 @@
       <c r="A226" s="3" t="s">
         <v>531</v>
       </c>
-      <c r="B226" s="0"/>
       <c r="C226" s="3" t="s">
         <v>532</v>
+      </c>
+    </row>
+    <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A227" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="C227" s="1" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A228" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C228" s="1" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A229" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="C229" s="1" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A230" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="C230" s="1" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A231" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="C231" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A232" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="B232" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A233" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="B233" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="C233" s="1" t="s">
+        <v>548</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More words - removed a comment.
</commit_message>
<xml_diff>
--- a/data/Words1.xlsx
+++ b/data/Words1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="576">
   <si>
     <t xml:space="preserve">Farsi</t>
   </si>
@@ -1654,6 +1654,12 @@
     <t xml:space="preserve">ما</t>
   </si>
   <si>
+    <t xml:space="preserve">ma </t>
+  </si>
+  <si>
+    <t xml:space="preserve">we </t>
+  </si>
+  <si>
     <t xml:space="preserve">شما</t>
   </si>
   <si>
@@ -1667,6 +1673,81 @@
   </si>
   <si>
     <t xml:space="preserve">they</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> همه چيز</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hame cheez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">everything</t>
+  </si>
+  <si>
+    <t xml:space="preserve">چیزی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cheezi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">something</t>
+  </si>
+  <si>
+    <t xml:space="preserve">هیچ چیز</t>
+  </si>
+  <si>
+    <t xml:space="preserve">heech cheez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nothing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">everyone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">کسی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kasi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">someone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">هیچکس</t>
+  </si>
+  <si>
+    <t xml:space="preserve">heechkas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">فارسی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">farsi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">انگلیسی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eengleesee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">چيز</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">فرد</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fard </t>
+  </si>
+  <si>
+    <t xml:space="preserve">person</t>
   </si>
 </sst>
 </file>
@@ -1753,24 +1834,24 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1790,15 +1871,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C233"/>
+  <dimension ref="A1:C243"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A222" colorId="64" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B233" activeCellId="0" sqref="B233"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A234" colorId="64" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B229" activeCellId="0" sqref="B229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="11.59"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="11.59"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="2" width="11.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1813,7 +1895,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1824,7 +1906,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1832,7 +1914,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1840,7 +1922,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -1848,7 +1930,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1856,7 +1938,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1864,7 +1946,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1872,7 +1954,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1880,7 +1962,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1888,7 +1970,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -1896,7 +1978,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1904,7 +1986,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1912,7 +1994,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1920,7 +2002,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -1928,7 +2010,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1936,7 +2018,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -1944,7 +2026,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -1952,7 +2034,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -1960,7 +2042,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -1968,7 +2050,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -1976,7 +2058,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1987,7 +2069,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -1995,7 +2077,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -2003,7 +2085,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -2011,7 +2093,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -2019,7 +2101,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -2027,7 +2109,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -2038,7 +2120,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -2046,7 +2128,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -2054,7 +2136,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="3" t="s">
         <v>63</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -2065,7 +2147,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="3" t="s">
         <v>66</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -2073,7 +2155,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="4" t="s">
         <v>68</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -2084,7 +2166,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="4" t="s">
         <v>71</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -2095,18 +2177,18 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="4" t="s">
         <v>77</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -2117,7 +2199,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="4" t="s">
         <v>80</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -2128,7 +2210,7 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="4" t="s">
         <v>80</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -2139,7 +2221,7 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="4" t="s">
         <v>84</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -2150,7 +2232,7 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="4" t="s">
         <v>87</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -2161,7 +2243,7 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="4" t="s">
         <v>90</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -2172,7 +2254,7 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="4" t="s">
         <v>93</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -2183,7 +2265,7 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="4" t="s">
         <v>96</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -2194,7 +2276,7 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="4" t="s">
         <v>99</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -2205,7 +2287,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="4" t="s">
         <v>102</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -2216,7 +2298,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="4" t="s">
         <v>105</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -2227,7 +2309,7 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="4" t="s">
         <v>108</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -2238,7 +2320,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="4" t="s">
         <v>111</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -2249,7 +2331,7 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="4" t="s">
         <v>114</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -2260,7 +2342,7 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="4" t="s">
         <v>117</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -2271,7 +2353,7 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="4" t="s">
         <v>119</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -2282,7 +2364,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="4" t="s">
         <v>122</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -2293,7 +2375,7 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="4" t="s">
         <v>125</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -2304,7 +2386,7 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="4" t="s">
         <v>128</v>
       </c>
       <c r="B54" s="1" t="s">
@@ -2315,7 +2397,7 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="4" t="s">
         <v>130</v>
       </c>
       <c r="B55" s="1" t="s">
@@ -2326,7 +2408,7 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="4" t="s">
         <v>133</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -2337,7 +2419,7 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="4" t="s">
         <v>136</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -2348,7 +2430,7 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="4" t="s">
         <v>133</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -2359,7 +2441,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="4" t="s">
         <v>139</v>
       </c>
       <c r="B59" s="1" t="s">
@@ -2370,7 +2452,7 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="3" t="s">
+      <c r="A60" s="4" t="s">
         <v>141</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -2381,7 +2463,7 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="3" t="s">
+      <c r="A61" s="4" t="s">
         <v>144</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -2392,7 +2474,7 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="3" t="s">
+      <c r="A62" s="4" t="s">
         <v>147</v>
       </c>
       <c r="B62" s="1" t="s">
@@ -2403,7 +2485,7 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="4" t="s">
         <v>150</v>
       </c>
       <c r="B63" s="1" t="s">
@@ -2414,7 +2496,7 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="3" t="s">
+      <c r="A64" s="4" t="s">
         <v>152</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -2425,7 +2507,7 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="3" t="s">
+      <c r="A65" s="4" t="s">
         <v>155</v>
       </c>
       <c r="B65" s="1" t="s">
@@ -2436,7 +2518,7 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="3" t="s">
+      <c r="A66" s="4" t="s">
         <v>158</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -2447,7 +2529,7 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="3" t="s">
+      <c r="A67" s="4" t="s">
         <v>161</v>
       </c>
       <c r="B67" s="1" t="s">
@@ -2458,7 +2540,7 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="3" t="s">
+      <c r="A68" s="4" t="s">
         <v>164</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -2469,7 +2551,7 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="3" t="s">
+      <c r="A69" s="4" t="s">
         <v>167</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -2480,7 +2562,7 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="3" t="s">
+      <c r="A70" s="4" t="s">
         <v>170</v>
       </c>
       <c r="B70" s="1" t="s">
@@ -2491,7 +2573,7 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="3" t="s">
+      <c r="A71" s="4" t="s">
         <v>164</v>
       </c>
       <c r="B71" s="1" t="s">
@@ -2502,7 +2584,7 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="3" t="s">
+      <c r="A72" s="4" t="s">
         <v>175</v>
       </c>
       <c r="B72" s="1" t="s">
@@ -2513,7 +2595,7 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="3" t="s">
+      <c r="A73" s="4" t="s">
         <v>178</v>
       </c>
       <c r="B73" s="1" t="s">
@@ -2524,7 +2606,7 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="3" t="s">
+      <c r="A74" s="4" t="s">
         <v>181</v>
       </c>
       <c r="B74" s="1" t="s">
@@ -2535,7 +2617,7 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="3" t="s">
+      <c r="A75" s="4" t="s">
         <v>184</v>
       </c>
       <c r="B75" s="1" t="s">
@@ -2546,7 +2628,7 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="3" t="s">
+      <c r="A76" s="4" t="s">
         <v>187</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -2557,7 +2639,7 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="3" t="s">
+      <c r="A77" s="4" t="s">
         <v>190</v>
       </c>
       <c r="B77" s="1" t="s">
@@ -2568,7 +2650,7 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="3" t="s">
+      <c r="A78" s="4" t="s">
         <v>193</v>
       </c>
       <c r="B78" s="1" t="s">
@@ -2579,7 +2661,7 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="3" t="s">
+      <c r="A79" s="4" t="s">
         <v>196</v>
       </c>
       <c r="B79" s="1" t="s">
@@ -2590,7 +2672,7 @@
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="3" t="s">
+      <c r="A80" s="4" t="s">
         <v>199</v>
       </c>
       <c r="B80" s="1" t="s">
@@ -2601,7 +2683,7 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="3" t="s">
+      <c r="A81" s="4" t="s">
         <v>187</v>
       </c>
       <c r="B81" s="1" t="s">
@@ -2612,7 +2694,7 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="3" t="s">
+      <c r="A82" s="4" t="s">
         <v>203</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -2623,7 +2705,7 @@
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="3" t="s">
+      <c r="A83" s="4" t="s">
         <v>205</v>
       </c>
       <c r="B83" s="1" t="s">
@@ -2634,7 +2716,7 @@
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="3" t="s">
+      <c r="A84" s="4" t="s">
         <v>187</v>
       </c>
       <c r="B84" s="1" t="s">
@@ -2645,7 +2727,7 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="3" t="s">
+      <c r="A85" s="4" t="s">
         <v>205</v>
       </c>
       <c r="B85" s="1" t="s">
@@ -2656,7 +2738,7 @@
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="3" t="s">
+      <c r="A86" s="4" t="s">
         <v>209</v>
       </c>
       <c r="B86" s="1" t="s">
@@ -2667,7 +2749,7 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="3" t="s">
+      <c r="A87" s="4" t="s">
         <v>212</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -2678,7 +2760,7 @@
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="3" t="s">
+      <c r="A88" s="4" t="s">
         <v>215</v>
       </c>
       <c r="B88" s="1" t="s">
@@ -2689,7 +2771,7 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="3" t="s">
+      <c r="A89" s="4" t="s">
         <v>218</v>
       </c>
       <c r="B89" s="1" t="s">
@@ -2700,7 +2782,7 @@
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="3" t="s">
+      <c r="A90" s="4" t="s">
         <v>221</v>
       </c>
       <c r="B90" s="1" t="s">
@@ -2711,7 +2793,7 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="3" t="s">
+      <c r="A91" s="4" t="s">
         <v>224</v>
       </c>
       <c r="B91" s="1" t="s">
@@ -2722,7 +2804,7 @@
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="3" t="s">
+      <c r="A92" s="4" t="s">
         <v>227</v>
       </c>
       <c r="B92" s="1" t="s">
@@ -2733,7 +2815,7 @@
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="3" t="s">
+      <c r="A93" s="4" t="s">
         <v>230</v>
       </c>
       <c r="B93" s="1" t="s">
@@ -2744,7 +2826,7 @@
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="3" t="s">
+      <c r="A94" s="4" t="s">
         <v>233</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -2755,7 +2837,7 @@
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="3" t="s">
+      <c r="A95" s="4" t="s">
         <v>236</v>
       </c>
       <c r="B95" s="1" t="s">
@@ -2766,7 +2848,7 @@
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="3" t="s">
+      <c r="A96" s="4" t="s">
         <v>239</v>
       </c>
       <c r="B96" s="1" t="s">
@@ -2777,7 +2859,7 @@
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="3" t="s">
+      <c r="A97" s="4" t="s">
         <v>242</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -2788,7 +2870,7 @@
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="3" t="s">
+      <c r="A98" s="4" t="s">
         <v>245</v>
       </c>
       <c r="B98" s="1" t="s">
@@ -2799,7 +2881,7 @@
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="3" t="s">
+      <c r="A99" s="4" t="s">
         <v>248</v>
       </c>
       <c r="B99" s="1" t="s">
@@ -2810,7 +2892,7 @@
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="3" t="s">
+      <c r="A100" s="4" t="s">
         <v>251</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -2821,7 +2903,7 @@
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="3" t="s">
+      <c r="A101" s="4" t="s">
         <v>254</v>
       </c>
       <c r="B101" s="1" t="s">
@@ -2832,7 +2914,7 @@
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="3" t="s">
+      <c r="A102" s="4" t="s">
         <v>257</v>
       </c>
       <c r="B102" s="1" t="s">
@@ -2843,7 +2925,7 @@
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="3" t="s">
+      <c r="A103" s="4" t="s">
         <v>260</v>
       </c>
       <c r="B103" s="1" t="s">
@@ -2854,7 +2936,7 @@
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="3" t="s">
+      <c r="A104" s="4" t="s">
         <v>263</v>
       </c>
       <c r="B104" s="1" t="s">
@@ -2865,7 +2947,7 @@
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="3" t="s">
+      <c r="A105" s="4" t="s">
         <v>266</v>
       </c>
       <c r="B105" s="1" t="s">
@@ -2876,7 +2958,7 @@
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="3" t="s">
+      <c r="A106" s="4" t="s">
         <v>269</v>
       </c>
       <c r="B106" s="1" t="s">
@@ -2887,7 +2969,7 @@
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="3" t="s">
+      <c r="A107" s="4" t="s">
         <v>272</v>
       </c>
       <c r="B107" s="1" t="s">
@@ -2898,7 +2980,7 @@
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A108" s="3" t="s">
+      <c r="A108" s="4" t="s">
         <v>275</v>
       </c>
       <c r="B108" s="1" t="s">
@@ -2909,7 +2991,7 @@
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="3" t="s">
+      <c r="A109" s="4" t="s">
         <v>278</v>
       </c>
       <c r="B109" s="1" t="s">
@@ -2920,7 +3002,7 @@
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="3" t="s">
+      <c r="A110" s="4" t="s">
         <v>281</v>
       </c>
       <c r="B110" s="1" t="s">
@@ -2931,7 +3013,7 @@
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="3" t="s">
+      <c r="A111" s="4" t="s">
         <v>284</v>
       </c>
       <c r="B111" s="1" t="s">
@@ -2942,7 +3024,7 @@
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="3" t="s">
+      <c r="A112" s="4" t="s">
         <v>287</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -2953,7 +3035,7 @@
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="3" t="s">
+      <c r="A113" s="4" t="s">
         <v>290</v>
       </c>
       <c r="B113" s="1" t="s">
@@ -2964,7 +3046,7 @@
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="3" t="s">
+      <c r="A114" s="4" t="s">
         <v>292</v>
       </c>
       <c r="B114" s="1" t="s">
@@ -2975,7 +3057,7 @@
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="3" t="s">
+      <c r="A115" s="4" t="s">
         <v>193</v>
       </c>
       <c r="B115" s="1" t="s">
@@ -2986,7 +3068,7 @@
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="3" t="s">
+      <c r="A116" s="4" t="s">
         <v>196</v>
       </c>
       <c r="B116" s="1" t="s">
@@ -2997,7 +3079,7 @@
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="3" t="s">
+      <c r="A117" s="4" t="s">
         <v>294</v>
       </c>
       <c r="B117" s="1" t="s">
@@ -3008,7 +3090,7 @@
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="3" t="s">
+      <c r="A118" s="4" t="s">
         <v>297</v>
       </c>
       <c r="B118" s="1" t="s">
@@ -3019,7 +3101,7 @@
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="3" t="s">
+      <c r="A119" s="4" t="s">
         <v>298</v>
       </c>
       <c r="B119" s="1" t="s">
@@ -3030,7 +3112,7 @@
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="3" t="s">
+      <c r="A120" s="4" t="s">
         <v>300</v>
       </c>
       <c r="B120" s="1" t="s">
@@ -3041,7 +3123,7 @@
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="3" t="s">
+      <c r="A121" s="4" t="s">
         <v>303</v>
       </c>
       <c r="B121" s="1" t="s">
@@ -3052,7 +3134,7 @@
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="3" t="s">
+      <c r="A122" s="4" t="s">
         <v>306</v>
       </c>
       <c r="B122" s="1" t="s">
@@ -3063,7 +3145,7 @@
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="3" t="s">
+      <c r="A123" s="4" t="s">
         <v>209</v>
       </c>
       <c r="B123" s="1" t="s">
@@ -3074,7 +3156,7 @@
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="3" t="s">
+      <c r="A124" s="4" t="s">
         <v>310</v>
       </c>
       <c r="B124" s="1" t="s">
@@ -3085,7 +3167,7 @@
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="3" t="s">
+      <c r="A125" s="4" t="s">
         <v>313</v>
       </c>
       <c r="B125" s="1" t="s">
@@ -3096,7 +3178,7 @@
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="3" t="s">
+      <c r="A126" s="4" t="s">
         <v>316</v>
       </c>
       <c r="B126" s="1" t="s">
@@ -3107,7 +3189,7 @@
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="3" t="s">
+      <c r="A127" s="4" t="s">
         <v>319</v>
       </c>
       <c r="B127" s="1" t="s">
@@ -3118,7 +3200,7 @@
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="3" t="s">
+      <c r="A128" s="4" t="s">
         <v>287</v>
       </c>
       <c r="B128" s="1" t="s">
@@ -3129,7 +3211,7 @@
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="3" t="s">
+      <c r="A129" s="4" t="s">
         <v>321</v>
       </c>
       <c r="B129" s="1" t="s">
@@ -3140,7 +3222,7 @@
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="3" t="s">
+      <c r="A130" s="4" t="s">
         <v>324</v>
       </c>
       <c r="B130" s="1" t="s">
@@ -3151,7 +3233,7 @@
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="3" t="s">
+      <c r="A131" s="4" t="s">
         <v>327</v>
       </c>
       <c r="B131" s="1" t="s">
@@ -3162,7 +3244,7 @@
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="3" t="s">
+      <c r="A132" s="4" t="s">
         <v>330</v>
       </c>
       <c r="B132" s="1" t="s">
@@ -3173,7 +3255,7 @@
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="3" t="s">
+      <c r="A133" s="4" t="s">
         <v>333</v>
       </c>
       <c r="B133" s="1" t="s">
@@ -3184,7 +3266,7 @@
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="3" t="s">
+      <c r="A134" s="4" t="s">
         <v>333</v>
       </c>
       <c r="B134" s="1" t="s">
@@ -3195,7 +3277,7 @@
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="3" t="s">
+      <c r="A135" s="4" t="s">
         <v>337</v>
       </c>
       <c r="B135" s="1" t="s">
@@ -3206,7 +3288,7 @@
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="3" t="s">
+      <c r="A136" s="4" t="s">
         <v>340</v>
       </c>
       <c r="B136" s="1" t="s">
@@ -3217,7 +3299,7 @@
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="3" t="s">
+      <c r="A137" s="4" t="s">
         <v>343</v>
       </c>
       <c r="B137" s="1" t="s">
@@ -3228,7 +3310,7 @@
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="3" t="s">
+      <c r="A138" s="4" t="s">
         <v>346</v>
       </c>
       <c r="B138" s="1" t="s">
@@ -3239,7 +3321,7 @@
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="3" t="s">
+      <c r="A139" s="4" t="s">
         <v>349</v>
       </c>
       <c r="B139" s="1" t="s">
@@ -3250,7 +3332,7 @@
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="3" t="s">
+      <c r="A140" s="4" t="s">
         <v>352</v>
       </c>
       <c r="B140" s="1" t="s">
@@ -3261,7 +3343,7 @@
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="3" t="s">
+      <c r="A141" s="4" t="s">
         <v>355</v>
       </c>
       <c r="B141" s="1" t="s">
@@ -3272,7 +3354,7 @@
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="3" t="s">
+      <c r="A142" s="4" t="s">
         <v>358</v>
       </c>
       <c r="B142" s="1" t="s">
@@ -3283,7 +3365,7 @@
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="3" t="s">
+      <c r="A143" s="4" t="s">
         <v>361</v>
       </c>
       <c r="B143" s="1" t="s">
@@ -3294,7 +3376,7 @@
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="3" t="s">
+      <c r="A144" s="4" t="s">
         <v>364</v>
       </c>
       <c r="B144" s="1" t="s">
@@ -3305,7 +3387,7 @@
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="3" t="s">
+      <c r="A145" s="4" t="s">
         <v>367</v>
       </c>
       <c r="B145" s="1" t="s">
@@ -3316,7 +3398,7 @@
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="3" t="s">
+      <c r="A146" s="4" t="s">
         <v>370</v>
       </c>
       <c r="B146" s="1" t="s">
@@ -3327,7 +3409,7 @@
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="3" t="s">
+      <c r="A147" s="4" t="s">
         <v>373</v>
       </c>
       <c r="B147" s="1" t="s">
@@ -3338,7 +3420,7 @@
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="3" t="s">
+      <c r="A148" s="4" t="s">
         <v>376</v>
       </c>
       <c r="B148" s="1" t="s">
@@ -3349,7 +3431,7 @@
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="3" t="s">
+      <c r="A149" s="4" t="s">
         <v>379</v>
       </c>
       <c r="B149" s="1" t="s">
@@ -3360,7 +3442,7 @@
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="3" t="s">
+      <c r="A150" s="4" t="s">
         <v>382</v>
       </c>
       <c r="B150" s="1" t="s">
@@ -3371,7 +3453,7 @@
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="3" t="s">
+      <c r="A151" s="4" t="s">
         <v>385</v>
       </c>
       <c r="B151" s="1" t="s">
@@ -3382,7 +3464,7 @@
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="3" t="s">
+      <c r="A152" s="4" t="s">
         <v>388</v>
       </c>
       <c r="B152" s="1" t="s">
@@ -3393,7 +3475,7 @@
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="3" t="s">
+      <c r="A153" s="4" t="s">
         <v>391</v>
       </c>
       <c r="B153" s="1" t="s">
@@ -3404,7 +3486,7 @@
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="3" t="s">
+      <c r="A154" s="4" t="s">
         <v>394</v>
       </c>
       <c r="B154" s="1" t="s">
@@ -3415,7 +3497,7 @@
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="3" t="s">
+      <c r="A155" s="4" t="s">
         <v>397</v>
       </c>
       <c r="B155" s="1" t="s">
@@ -3426,7 +3508,7 @@
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="3" t="s">
+      <c r="A156" s="4" t="s">
         <v>400</v>
       </c>
       <c r="B156" s="1" t="s">
@@ -3438,567 +3520,567 @@
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="3" t="s">
+      <c r="A157" s="4" t="s">
         <v>402</v>
       </c>
-      <c r="C157" s="3" t="s">
+      <c r="C157" s="4" t="s">
         <v>403</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="3" t="s">
+      <c r="A158" s="4" t="s">
         <v>404</v>
       </c>
-      <c r="C158" s="3" t="s">
+      <c r="C158" s="4" t="s">
         <v>405</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="3" t="s">
+      <c r="A159" s="4" t="s">
         <v>406</v>
       </c>
-      <c r="C159" s="3" t="s">
+      <c r="C159" s="4" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="3" t="s">
+      <c r="A160" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="C160" s="3" t="s">
+      <c r="C160" s="4" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="3" t="s">
+      <c r="A161" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="C161" s="3" t="s">
+      <c r="C161" s="4" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="3" t="s">
+      <c r="A162" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="C162" s="3" t="s">
+      <c r="C162" s="4" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="3" t="s">
+      <c r="A163" s="4" t="s">
         <v>414</v>
       </c>
-      <c r="C163" s="3" t="s">
+      <c r="C163" s="4" t="s">
         <v>415</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="3" t="s">
+      <c r="A164" s="4" t="s">
         <v>416</v>
       </c>
-      <c r="C164" s="3" t="s">
+      <c r="C164" s="4" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="3" t="s">
+      <c r="A165" s="4" t="s">
         <v>418</v>
       </c>
-      <c r="C165" s="3" t="s">
+      <c r="C165" s="4" t="s">
         <v>419</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="3" t="s">
+      <c r="A166" s="4" t="s">
         <v>420</v>
       </c>
-      <c r="C166" s="3" t="s">
+      <c r="C166" s="4" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="3" t="s">
+      <c r="A167" s="4" t="s">
         <v>422</v>
       </c>
-      <c r="C167" s="3" t="s">
+      <c r="C167" s="4" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="3" t="s">
+      <c r="A168" s="4" t="s">
         <v>424</v>
       </c>
-      <c r="C168" s="3" t="s">
+      <c r="C168" s="4" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="3" t="s">
+      <c r="A169" s="4" t="s">
         <v>426</v>
       </c>
-      <c r="C169" s="3" t="s">
+      <c r="C169" s="4" t="s">
         <v>427</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="3" t="s">
+      <c r="A170" s="4" t="s">
         <v>428</v>
       </c>
-      <c r="C170" s="3" t="s">
+      <c r="C170" s="4" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="3" t="s">
+      <c r="A171" s="4" t="s">
         <v>430</v>
       </c>
-      <c r="C171" s="3" t="s">
+      <c r="C171" s="4" t="s">
         <v>431</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="3" t="s">
+      <c r="A172" s="4" t="s">
         <v>432</v>
       </c>
-      <c r="C172" s="3" t="s">
+      <c r="C172" s="4" t="s">
         <v>433</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="3" t="s">
+      <c r="A173" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="C173" s="3" t="s">
+      <c r="C173" s="4" t="s">
         <v>435</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="3" t="s">
+      <c r="A174" s="4" t="s">
         <v>436</v>
       </c>
-      <c r="C174" s="3" t="s">
+      <c r="C174" s="4" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="3" t="s">
+      <c r="A175" s="4" t="s">
         <v>438</v>
       </c>
-      <c r="C175" s="3" t="s">
+      <c r="C175" s="4" t="s">
         <v>439</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="3" t="s">
+      <c r="A176" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="C176" s="3" t="s">
+      <c r="C176" s="4" t="s">
         <v>440</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="3" t="s">
+      <c r="A177" s="4" t="s">
         <v>441</v>
       </c>
-      <c r="C177" s="3" t="s">
+      <c r="C177" s="4" t="s">
         <v>442</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="3" t="s">
+      <c r="A178" s="4" t="s">
         <v>443</v>
       </c>
-      <c r="C178" s="3" t="s">
+      <c r="C178" s="4" t="s">
         <v>444</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="3" t="s">
+      <c r="A179" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="C179" s="3" t="s">
+      <c r="C179" s="4" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="3" t="s">
+      <c r="A180" s="4" t="s">
         <v>447</v>
       </c>
-      <c r="C180" s="3" t="s">
+      <c r="C180" s="4" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="3" t="s">
+      <c r="A181" s="4" t="s">
         <v>449</v>
       </c>
-      <c r="C181" s="3" t="s">
+      <c r="C181" s="4" t="s">
         <v>450</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="3" t="s">
+      <c r="A182" s="4" t="s">
         <v>451</v>
       </c>
-      <c r="C182" s="3" t="s">
+      <c r="C182" s="4" t="s">
         <v>452</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="3" t="s">
+      <c r="A183" s="4" t="s">
         <v>453</v>
       </c>
-      <c r="C183" s="3" t="s">
+      <c r="C183" s="4" t="s">
         <v>454</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="3" t="s">
+      <c r="A184" s="4" t="s">
         <v>455</v>
       </c>
-      <c r="C184" s="3" t="s">
+      <c r="C184" s="4" t="s">
         <v>456</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="3" t="s">
+      <c r="A185" s="4" t="s">
         <v>457</v>
       </c>
-      <c r="C185" s="3" t="s">
+      <c r="C185" s="4" t="s">
         <v>458</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="3" t="s">
+      <c r="A186" s="4" t="s">
         <v>459</v>
       </c>
-      <c r="C186" s="3" t="s">
+      <c r="C186" s="4" t="s">
         <v>460</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="3" t="s">
+      <c r="A187" s="4" t="s">
         <v>461</v>
       </c>
-      <c r="C187" s="3" t="s">
+      <c r="C187" s="4" t="s">
         <v>462</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="3" t="s">
+      <c r="A188" s="4" t="s">
         <v>463</v>
       </c>
-      <c r="C188" s="3" t="s">
+      <c r="C188" s="4" t="s">
         <v>464</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="3" t="s">
+      <c r="A189" s="4" t="s">
         <v>465</v>
       </c>
-      <c r="C189" s="3" t="s">
+      <c r="C189" s="4" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="3" t="s">
+      <c r="A190" s="4" t="s">
         <v>467</v>
       </c>
-      <c r="C190" s="3" t="s">
+      <c r="C190" s="4" t="s">
         <v>468</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="3" t="s">
+      <c r="A191" s="4" t="s">
         <v>469</v>
       </c>
-      <c r="C191" s="3" t="s">
+      <c r="C191" s="4" t="s">
         <v>470</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="3" t="s">
+      <c r="A192" s="4" t="s">
         <v>471</v>
       </c>
-      <c r="C192" s="3" t="s">
+      <c r="C192" s="4" t="s">
         <v>472</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="3" t="s">
+      <c r="A193" s="4" t="s">
         <v>473</v>
       </c>
-      <c r="C193" s="3" t="s">
+      <c r="C193" s="4" t="s">
         <v>474</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="3" t="s">
+      <c r="A194" s="4" t="s">
         <v>475</v>
       </c>
-      <c r="C194" s="3" t="s">
+      <c r="C194" s="4" t="s">
         <v>476</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="3" t="s">
+      <c r="A195" s="4" t="s">
         <v>477</v>
       </c>
-      <c r="C195" s="3" t="s">
+      <c r="C195" s="4" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="3" t="s">
+      <c r="A196" s="4" t="s">
         <v>479</v>
       </c>
-      <c r="C196" s="3" t="s">
+      <c r="C196" s="4" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="3" t="s">
+      <c r="A197" s="4" t="s">
         <v>481</v>
       </c>
-      <c r="C197" s="3" t="s">
+      <c r="C197" s="4" t="s">
         <v>482</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="3" t="s">
+      <c r="A198" s="4" t="s">
         <v>483</v>
       </c>
-      <c r="C198" s="3" t="s">
+      <c r="C198" s="4" t="s">
         <v>484</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="3" t="s">
+      <c r="A199" s="4" t="s">
         <v>485</v>
       </c>
-      <c r="C199" s="3" t="s">
+      <c r="C199" s="4" t="s">
         <v>486</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="3" t="s">
+      <c r="A200" s="4" t="s">
         <v>487</v>
       </c>
-      <c r="C200" s="3" t="s">
+      <c r="C200" s="4" t="s">
         <v>488</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="3" t="s">
+      <c r="A201" s="4" t="s">
         <v>489</v>
       </c>
-      <c r="C201" s="3" t="s">
+      <c r="C201" s="4" t="s">
         <v>490</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="3" t="s">
+      <c r="A202" s="4" t="s">
         <v>491</v>
       </c>
-      <c r="C202" s="3" t="s">
+      <c r="C202" s="4" t="s">
         <v>492</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="3" t="s">
+      <c r="A203" s="4" t="s">
         <v>493</v>
       </c>
-      <c r="C203" s="3" t="s">
+      <c r="C203" s="4" t="s">
         <v>494</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="3" t="s">
+      <c r="A204" s="4" t="s">
         <v>495</v>
       </c>
-      <c r="C204" s="3" t="s">
+      <c r="C204" s="4" t="s">
         <v>496</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="3" t="s">
+      <c r="A205" s="4" t="s">
         <v>497</v>
       </c>
-      <c r="C205" s="3" t="s">
+      <c r="C205" s="4" t="s">
         <v>498</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="3" t="s">
+      <c r="A206" s="4" t="s">
         <v>499</v>
       </c>
-      <c r="C206" s="3" t="s">
+      <c r="C206" s="4" t="s">
         <v>500</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="3" t="s">
+      <c r="A207" s="4" t="s">
         <v>501</v>
       </c>
-      <c r="C207" s="3" t="s">
+      <c r="C207" s="4" t="s">
         <v>502</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="3" t="s">
+      <c r="A208" s="4" t="s">
         <v>503</v>
       </c>
-      <c r="C208" s="3" t="s">
+      <c r="C208" s="4" t="s">
         <v>504</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="3" t="s">
+      <c r="A209" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="C209" s="3" t="s">
+      <c r="C209" s="4" t="s">
         <v>505</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="3" t="s">
+      <c r="A210" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C210" s="3" t="s">
+      <c r="C210" s="4" t="s">
         <v>506</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="3" t="s">
+      <c r="A211" s="4" t="s">
         <v>507</v>
       </c>
-      <c r="C211" s="3" t="s">
+      <c r="C211" s="4" t="s">
         <v>508</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A212" s="3" t="s">
+      <c r="A212" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="C212" s="3" t="s">
+      <c r="C212" s="4" t="s">
         <v>509</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A213" s="3" t="s">
+      <c r="A213" s="4" t="s">
         <v>510</v>
       </c>
-      <c r="C213" s="3" t="s">
+      <c r="C213" s="4" t="s">
         <v>511</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A214" s="3" t="s">
+      <c r="A214" s="4" t="s">
         <v>512</v>
       </c>
-      <c r="C214" s="3" t="s">
+      <c r="C214" s="4" t="s">
         <v>513</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="3" t="s">
+      <c r="A215" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="C215" s="3" t="s">
+      <c r="C215" s="4" t="s">
         <v>514</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="3" t="s">
+      <c r="A216" s="4" t="s">
         <v>515</v>
       </c>
-      <c r="C216" s="3" t="s">
+      <c r="C216" s="4" t="s">
         <v>516</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A217" s="3" t="s">
+      <c r="A217" s="4" t="s">
         <v>517</v>
       </c>
-      <c r="C217" s="3" t="s">
+      <c r="C217" s="4" t="s">
         <v>518</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A218" s="3" t="s">
+      <c r="A218" s="4" t="s">
         <v>519</v>
       </c>
-      <c r="C218" s="3" t="s">
+      <c r="C218" s="4" t="s">
         <v>520</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A219" s="3" t="s">
+      <c r="A219" s="4" t="s">
         <v>521</v>
       </c>
-      <c r="C219" s="3" t="s">
+      <c r="C219" s="4" t="s">
         <v>522</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A220" s="3" t="s">
+      <c r="A220" s="4" t="s">
         <v>523</v>
       </c>
-      <c r="C220" s="3" t="s">
+      <c r="C220" s="4" t="s">
         <v>524</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A221" s="3" t="s">
+      <c r="A221" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="C221" s="3" t="s">
+      <c r="C221" s="4" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A222" s="3" t="s">
+      <c r="A222" s="4" t="s">
         <v>394</v>
       </c>
-      <c r="C222" s="3" t="s">
+      <c r="C222" s="4" t="s">
         <v>526</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A223" s="3" t="s">
+      <c r="A223" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="C223" s="3" t="s">
+      <c r="C223" s="4" t="s">
         <v>527</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="3" t="s">
+      <c r="A224" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C224" s="3" t="s">
+      <c r="C224" s="4" t="s">
         <v>528</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A225" s="3" t="s">
+      <c r="A225" s="4" t="s">
         <v>529</v>
       </c>
-      <c r="C225" s="3" t="s">
+      <c r="C225" s="4" t="s">
         <v>530</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A226" s="3" t="s">
+      <c r="A226" s="4" t="s">
         <v>531</v>
       </c>
-      <c r="C226" s="3" t="s">
+      <c r="C226" s="4" t="s">
         <v>532</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A227" s="3" t="s">
+      <c r="A227" s="4" t="s">
         <v>533</v>
       </c>
       <c r="B227" s="1" t="s">
@@ -4009,7 +4091,7 @@
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A228" s="3" t="s">
+      <c r="A228" s="4" t="s">
         <v>139</v>
       </c>
       <c r="B228" s="1" t="s">
@@ -4020,7 +4102,7 @@
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="3" t="s">
+      <c r="A229" s="4" t="s">
         <v>537</v>
       </c>
       <c r="B229" s="1" t="s">
@@ -4031,7 +4113,7 @@
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A230" s="3" t="s">
+      <c r="A230" s="4" t="s">
         <v>540</v>
       </c>
       <c r="B230" s="1" t="s">
@@ -4042,36 +4124,146 @@
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A231" s="3" t="s">
+      <c r="A231" s="4" t="s">
         <v>543</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>534</v>
+        <v>544</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>305</v>
+        <v>545</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A232" s="3" t="s">
-        <v>544</v>
+      <c r="A232" s="4" t="s">
+        <v>546</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A233" s="3" t="s">
-        <v>546</v>
+      <c r="A233" s="4" t="s">
+        <v>548</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>548</v>
+        <v>550</v>
+      </c>
+    </row>
+    <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A234" s="4" t="s">
+        <v>551</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="C234" s="4" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A235" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="C235" s="1" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A236" s="4" t="s">
+        <v>557</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A237" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B237" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A238" s="4" t="s">
+        <v>561</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A239" s="4" t="s">
+        <v>564</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A240" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A241" s="4" t="s">
+        <v>569</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="C241" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A242" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="B242" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="C242" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A243" s="4" t="s">
+        <v>573</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>575</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding more words from today's lessons - up to 252!
</commit_message>
<xml_diff>
--- a/data/Words1.xlsx
+++ b/data/Words1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="600">
   <si>
     <t xml:space="preserve">Farsi</t>
   </si>
@@ -1748,6 +1748,78 @@
   </si>
   <si>
     <t xml:space="preserve">person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">انجام</t>
+  </si>
+  <si>
+    <t xml:space="preserve">anjam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">قرار</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gherar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">appointment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">محل</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mahl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">فوق </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Above</t>
+  </si>
+  <si>
+    <t xml:space="preserve">العاده</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extraordinary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">می گردیم</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We return</t>
+  </si>
+  <si>
+    <t xml:space="preserve">تشنه</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tashneh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thirsty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">واقع</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indeed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">بخوانم</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I read</t>
+  </si>
+  <si>
+    <t xml:space="preserve">نام</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nam(eh)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
   </si>
 </sst>
 </file>
@@ -1871,10 +1943,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C243"/>
+  <dimension ref="A1:C253"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A234" colorId="64" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B229" activeCellId="0" sqref="B229"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A240" colorId="64" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B252" activeCellId="0" sqref="B252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4266,6 +4338,101 @@
         <v>575</v>
       </c>
     </row>
+    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A244" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="C244" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A245" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="C245" s="1" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A246" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A247" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A248" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="C248" s="1" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="C249" s="1" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A250" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="B250" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="C250" s="1" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A251" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="C251" s="1" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A252" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="C252" s="1" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A253" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>599</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Proper game length settings - adding pronunciation in the guess.
</commit_message>
<xml_diff>
--- a/data/Words1.xlsx
+++ b/data/Words1.xlsx
@@ -2268,7 +2268,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2295,11 +2295,6 @@
       <name val="Lohit Devanagari"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2344,7 +2339,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2373,10 +2368,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2396,8 +2387,8 @@
   </sheetPr>
   <dimension ref="A1:C306"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A288" colorId="64" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B307" activeCellId="0" sqref="B307"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5138,7 +5129,7 @@
       </c>
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A277" s="7" t="s">
+      <c r="A277" s="6" t="s">
         <v>660</v>
       </c>
       <c r="B277" s="1" t="s">

</xml_diff>

<commit_message>
Additional words for tonight!
</commit_message>
<xml_diff>
--- a/data/Words1.xlsx
+++ b/data/Words1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="746">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="808">
   <si>
     <t xml:space="preserve">Farsi</t>
   </si>
@@ -2258,6 +2258,192 @@
   </si>
   <si>
     <t xml:space="preserve">come</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raftan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cleave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">برگشتن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bargashtan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">return</t>
+  </si>
+  <si>
+    <t xml:space="preserve">دادن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dadan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">give</t>
+  </si>
+  <si>
+    <t xml:space="preserve">برداشتن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bardashtan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">take</t>
+  </si>
+  <si>
+    <t xml:space="preserve">آوردن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avardan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">دنبال __ گشتن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Donbale __ gashtan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">look for</t>
+  </si>
+  <si>
+    <t xml:space="preserve">پیدا کردن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">peyda kardan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">find</t>
+  </si>
+  <si>
+    <t xml:space="preserve">گرفتن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gereftan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">get </t>
+  </si>
+  <si>
+    <t xml:space="preserve">receive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">خريدن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">khareedan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> امتحان کردن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emtehan kardan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">try</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شروع کردن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shoroo’ cardan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">دیگر </t>
+  </si>
+  <si>
+    <t xml:space="preserve">stop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!دیگر نخور</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deegar nakhor!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stop eating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">تمام کردن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tamam kardan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ادامه دادن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edame dadan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">continue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">بیدار شدن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beedar shodan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wake up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">پا شدن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pa shodan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">get up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">خوردن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">khordan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">اتفاق افتادن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Et-tefagh oftadan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">happen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">احساس کردن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ehsas kardan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">feel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">درست کردن  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dorost kardan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">create/make</t>
   </si>
 </sst>
 </file>
@@ -2268,7 +2454,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2293,6 +2479,13 @@
     <font>
       <sz val="10"/>
       <name val="Lohit Devanagari"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -2339,7 +2532,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2368,6 +2561,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2385,10 +2582,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C306"/>
+  <dimension ref="A1:C328"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A306" colorId="64" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C329" activeCellId="0" sqref="C329"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5458,6 +5655,248 @@
         <v>745</v>
       </c>
     </row>
+    <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A307" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B307" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="C307" s="1" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A308" s="7" t="s">
+        <v>748</v>
+      </c>
+      <c r="B308" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="C308" s="1" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A309" s="7" t="s">
+        <v>751</v>
+      </c>
+      <c r="B309" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="C309" s="1" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A310" s="7" t="s">
+        <v>754</v>
+      </c>
+      <c r="B310" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="C310" s="1" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A311" s="7" t="s">
+        <v>757</v>
+      </c>
+      <c r="B311" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="C311" s="1" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A312" s="7" t="s">
+        <v>760</v>
+      </c>
+      <c r="B312" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="C312" s="1" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A313" s="7" t="s">
+        <v>763</v>
+      </c>
+      <c r="B313" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="C313" s="1" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A314" s="7" t="s">
+        <v>766</v>
+      </c>
+      <c r="B314" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="C314" s="1" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A315" s="7" t="s">
+        <v>766</v>
+      </c>
+      <c r="B315" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="C315" s="1" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A316" s="7" t="s">
+        <v>770</v>
+      </c>
+      <c r="B316" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="C316" s="1" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A317" s="7" t="s">
+        <v>773</v>
+      </c>
+      <c r="B317" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="C317" s="1" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A318" s="7" t="s">
+        <v>776</v>
+      </c>
+      <c r="B318" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="C318" s="1" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A319" s="7" t="s">
+        <v>779</v>
+      </c>
+      <c r="B319" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C319" s="1" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A320" s="7" t="s">
+        <v>781</v>
+      </c>
+      <c r="B320" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="C320" s="1" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A321" s="7" t="s">
+        <v>784</v>
+      </c>
+      <c r="B321" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="C321" s="1" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A322" s="7" t="s">
+        <v>787</v>
+      </c>
+      <c r="B322" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="C322" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A323" s="7" t="s">
+        <v>790</v>
+      </c>
+      <c r="B323" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="C323" s="1" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A324" s="7" t="s">
+        <v>793</v>
+      </c>
+      <c r="B324" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="C324" s="1" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A325" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="B325" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="C325" s="1" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A326" s="7" t="s">
+        <v>799</v>
+      </c>
+      <c r="B326" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="C326" s="1" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A327" s="7" t="s">
+        <v>802</v>
+      </c>
+      <c r="B327" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="C327" s="1" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A328" s="7" t="s">
+        <v>805</v>
+      </c>
+      <c r="B328" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="C328" s="1" t="s">
+        <v>807</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added a cool 'word'
</commit_message>
<xml_diff>
--- a/data/Words1.xlsx
+++ b/data/Words1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="808">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="811">
   <si>
     <t xml:space="preserve">Farsi</t>
   </si>
@@ -2444,6 +2444,15 @@
   </si>
   <si>
     <t xml:space="preserve">create/make</t>
+  </si>
+  <si>
+    <t xml:space="preserve">جا به جا</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ja beh ja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">displaced</t>
   </si>
 </sst>
 </file>
@@ -2582,9 +2591,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C328"/>
+  <dimension ref="A1:C329"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A306" colorId="64" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A322" colorId="64" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C329" activeCellId="0" sqref="C329"/>
     </sheetView>
   </sheetViews>
@@ -5897,6 +5906,17 @@
         <v>807</v>
       </c>
     </row>
+    <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A329" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="B329" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="C329" s="1" t="s">
+        <v>810</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>